<commit_message>
fixed #536 FlixelRL-536 画像表示コマンド(IMAGE)を実装する
</commit_message>
<xml_diff>
--- a/docs/event.xlsx
+++ b/docs/event.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -85,8 +85,10 @@
     <t>「これは……、もしかして宝石がたくさん詰まったお宝？！」</t>
   </si>
   <si>
-    <t>女の子はドキドキして宝箱を開きます。&lt;br&gt;
-しかし、中にあるのは小さなマタタビの木でした。</t>
+    <t>女の子はドキドキして宝箱を開きます。</t>
+  </si>
+  <si>
+    <t>しかし、中にあるのは小さなマタタビの木でした。</t>
   </si>
   <si>
     <t>「……」</t>
@@ -1472,7 +1474,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1661,7 +1663,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" ht="29.95" customHeight="1">
+    <row r="25" ht="20" customHeight="1">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1685,7 +1687,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" ht="44.95" customHeight="1">
+    <row r="28" ht="20" customHeight="1">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" ht="29.95" customHeight="1">
+    <row r="31" ht="20" customHeight="1">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -1723,6 +1725,14 @@
       </c>
       <c r="B32" t="s" s="4">
         <v>26</v>
+      </c>
+    </row>
+    <row r="33" ht="20" customHeight="1">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s" s="4">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>